<commit_message>
Fixed issues discovered in first build
- fixed potentiometer footprint
- bigger strain relief holes: .1” to .15”
- changed value of C9 (AC coupling capacitor) to 22uF in BOM and
schematic
- Removed R8 (jumper to bypass op amp)
- Increased length of surface mount pads for 0805 components to
facilitate hand soldering
- Regenerated gerbers, jpg previews, and pdf of schematic
</commit_message>
<xml_diff>
--- a/SI4825_KIT_SMT_BOM.xlsx
+++ b/SI4825_KIT_SMT_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgb/Desktop/SI4825_kit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgb/Documents/github/Si4825-AM-FM-Radio-Kit-SMT/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
   <si>
     <t>Ref Des</t>
   </si>
@@ -47,15 +47,6 @@
     <t>C1, C2</t>
   </si>
   <si>
-    <t>22pF 0805 Capacitor</t>
-  </si>
-  <si>
-    <t>C3-C7</t>
-  </si>
-  <si>
-    <t>1uF 0805 Capacitor</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -270,6 +261,45 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>C3-C6, C8</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/murata-electronics-north-america/GRM21BC80G226ME39L/490-6464-1-ND/3845661</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM21BC80G226ME39L</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>CC0805KKX7R7BB105</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>C0805C220J5GACTU</t>
+  </si>
+  <si>
+    <t>22pF 0805 C0G Capacitor</t>
+  </si>
+  <si>
+    <t>1uF 0805 X7R Capacitor</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>22uF 0805 X6S Capacitor</t>
+  </si>
+  <si>
+    <t>NOSTUFF</t>
   </si>
 </sst>
 </file>
@@ -585,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -615,13 +645,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -629,7 +659,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -638,15 +674,21 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -655,126 +697,129 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>8.3999999999999995E-3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>2.1000000000000001E-2</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -783,18 +828,18 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -803,199 +848,219 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>2.1749999999999998</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="1">
-        <v>1.7999999999999999E-2</v>
+      <c r="F13">
+        <v>2.1749999999999998</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>8.7999999999999995E-2</v>
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15">
-        <v>0.55900000000000005</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" t="s">
-        <v>80</v>
+      <c r="F16">
+        <v>0.55900000000000005</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>0.33</v>
+      <c r="F17" t="s">
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>2.14</v>
+        <v>0.2</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2.14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>